<commit_message>
Update Rev 2 Files
</commit_message>
<xml_diff>
--- a/Hardware/Rev 2/ARK Flow Rev 2 BOM.xlsx
+++ b/Hardware/Rev 2/ARK Flow Rev 2 BOM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="216">
   <si>
     <t>LibRef</t>
   </si>
@@ -363,7 +363,7 @@
     <t>30327</t>
   </si>
   <si>
-    <t>R4, R6, R10, R13, R15, R17, R18</t>
+    <t>R4, R6, R10, R13, R15, R17</t>
   </si>
   <si>
     <t>AC0402JR-070RL</t>
@@ -648,25 +648,22 @@
     <t>516-AFBR-S50LV85D-ND</t>
   </si>
   <si>
-    <t>30935</t>
+    <t>31021</t>
   </si>
   <si>
     <t>U9</t>
   </si>
   <si>
-    <t>Bosch Sensortec</t>
-  </si>
-  <si>
-    <t>BMI088</t>
-  </si>
-  <si>
-    <t>ACCELEROMETER 16LGA</t>
-  </si>
-  <si>
-    <t>BMI055</t>
-  </si>
-  <si>
-    <t>828-1082-2-ND</t>
+    <t>TDK InvenSense</t>
+  </si>
+  <si>
+    <t>ICM-42688-P</t>
+  </si>
+  <si>
+    <t>MOTION SENSOR</t>
+  </si>
+  <si>
+    <t>1428-ICM-42688-PTR-ND</t>
   </si>
 </sst>
 </file>
@@ -1480,7 +1477,7 @@
         <v>115</v>
       </c>
       <c r="C17" s="17">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D17" s="16" t="s">
         <v>108</v>
@@ -1975,13 +1972,13 @@
         <v>214</v>
       </c>
       <c r="H32" s="16" t="s">
+        <v>213</v>
+      </c>
+      <c r="I32" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="J32" s="16" t="s">
         <v>215</v>
-      </c>
-      <c r="I32" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="J32" s="16" t="s">
-        <v>216</v>
       </c>
     </row>
   </sheetData>

</xml_diff>